<commit_message>
Added ASCII check to WebScrapper, new categories
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="511">
   <si>
     <t>link</t>
   </si>
@@ -1595,6 +1595,18 @@
   </si>
   <si>
     <t>http://net-informations.com/faq/default.htm</t>
+  </si>
+  <si>
+    <t>https://www.washingtonpost.com/politics/challenges-have-dogged-obamas-health-plan-since-2010/2013/11/02/453fba42-426b-11e3-a624-41d661b0bb78_print.html?</t>
+  </si>
+  <si>
+    <t>http://nymag.com/daily/intelligencer/2013/11/how-i-learned-to-love-twitter.html</t>
+  </si>
+  <si>
+    <t>https://www.theawl.com/2015/12/access-denied/</t>
+  </si>
+  <si>
+    <t>https://www.vqronline.org/essays-articles/2016/07/mysterious-american-cat</t>
   </si>
 </sst>
 </file>
@@ -1946,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F501"/>
+  <dimension ref="A1:F505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A483" workbookViewId="0">
-      <selection activeCell="A487" sqref="A487"/>
+    <sheetView tabSelected="1" topLeftCell="A484" workbookViewId="0">
+      <selection activeCell="A504" sqref="A504:B505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5970,6 +5982,38 @@
       </c>
       <c r="B501" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>507</v>
+      </c>
+      <c r="B502" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>508</v>
+      </c>
+      <c r="B503" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B504" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>510</v>
+      </c>
+      <c r="B505" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -5991,8 +6035,9 @@
     <hyperlink ref="A26" r:id="rId15"/>
     <hyperlink ref="A12" r:id="rId16"/>
     <hyperlink ref="A88" r:id="rId17"/>
+    <hyperlink ref="A504" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New categories, made the  ER errorproof, dramatic mode
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="527">
   <si>
     <t>link</t>
   </si>
@@ -1608,12 +1608,60 @@
   <si>
     <t>https://www.vqronline.org/essays-articles/2016/07/mysterious-american-cat</t>
   </si>
+  <si>
+    <t>https://medium.com/content-uneditable/circular-dependencies-in-javascript-a-k-a-coding-is-not-a-rock-paper-scissors-game-9c2a9eccd4bc</t>
+  </si>
+  <si>
+    <t>https://medium.com/javascript-scene/inside-the-dev-team-death-spiral-6a7ea255467b</t>
+  </si>
+  <si>
+    <t>https://qz.com/1285418/giant-predatory-worms-from-asia-are-invading-france/?utm_source=parAO</t>
+  </si>
+  <si>
+    <t>https://sexier.com/live-sex-chats/?queryid=138</t>
+  </si>
+  <si>
+    <t>https://vividcams.com/?AFNO=MjAyOTEzLjU0LjQ2LjEwMi4xOS4wLjAuMC4w&amp;mobile=0&amp;nats=MjAyOTEzLjU0LjQ2LjEwMi4xOS4wLjAuMC4w&amp;strack=0&amp;switched=1</t>
+  </si>
+  <si>
+    <t>https://cams.com/go/g1424946-pct</t>
+  </si>
+  <si>
+    <t>http://myporncams.com/</t>
+  </si>
+  <si>
+    <t>https://livecam-experts.com/</t>
+  </si>
+  <si>
+    <t>https://www.xlovecam.com/en/</t>
+  </si>
+  <si>
+    <t>https://www.flirt4free.com/live/girls/</t>
+  </si>
+  <si>
+    <t>https://www.pornication.com/?AFNO=1-247331-2-2-bestxxxsites</t>
+  </si>
+  <si>
+    <t>https://www.myfreecams.com/?cam=30546&amp;omp=2&amp;track=102c530982c0f2496e5886e66ee166&amp;skip_oapopup=1&amp;r=0&amp;mfwd=1#{model}</t>
+  </si>
+  <si>
+    <t>https://www.privatefeeds.com/?AFNO=1-247331-2-bestxxxsites</t>
+  </si>
+  <si>
+    <t>https://www.streamate.com/?AFNO=1-0-642160-356079&amp;DF=0&amp;UHNSMTY=303</t>
+  </si>
+  <si>
+    <t>https://www.evilangellive.com/?AFNO=1-247331-2-2-bestxxxsites</t>
+  </si>
+  <si>
+    <t>https://www.watchmygf.me/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1648,6 +1696,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1670,11 +1725,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1958,10 +2016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F505"/>
+  <dimension ref="A1:F521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A484" workbookViewId="0">
-      <selection activeCell="A504" sqref="A504:B505"/>
+    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
+      <selection activeCell="A521" sqref="A521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6014,6 +6072,134 @@
       </c>
       <c r="B505" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>511</v>
+      </c>
+      <c r="B506" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A507" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B507" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>513</v>
+      </c>
+      <c r="B508" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>514</v>
+      </c>
+      <c r="B509" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>515</v>
+      </c>
+      <c r="B510" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>516</v>
+      </c>
+      <c r="B511" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>517</v>
+      </c>
+      <c r="B512" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>519</v>
+      </c>
+      <c r="B513" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>518</v>
+      </c>
+      <c r="B514" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>520</v>
+      </c>
+      <c r="B515" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>521</v>
+      </c>
+      <c r="B516" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>522</v>
+      </c>
+      <c r="B517" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>523</v>
+      </c>
+      <c r="B518" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>524</v>
+      </c>
+      <c r="B519" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>525</v>
+      </c>
+      <c r="B520" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>526</v>
+      </c>
+      <c r="B521" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes before CR 2
</commit_message>
<xml_diff>
--- a/Categories.xlsx
+++ b/Categories.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="515">
   <si>
     <t>link</t>
   </si>
@@ -1616,6 +1616,9 @@
   </si>
   <si>
     <t>https://www.theguardian.com/science/2018/may/30/speculative-biology-understanding-the-past-and-predicting-our-future</t>
+  </si>
+  <si>
+    <t>https://likegeeks.com/python-gui-examples-tkinter-tutorial/</t>
   </si>
 </sst>
 </file>
@@ -1977,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F511"/>
+  <dimension ref="A1:F512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="A395" sqref="A395:B511"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A502" sqref="A502"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6057,6 +6060,14 @@
       </c>
       <c r="B511" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>514</v>
+      </c>
+      <c r="B512" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>